<commit_message>
added xl sheet order
</commit_message>
<xml_diff>
--- a/DataFile/Data.xlsx
+++ b/DataFile/Data.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Login_App" sheetId="1" r:id="rId1"/>
+    <sheet name="Buy" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Login_App</t>
-  </si>
-  <si>
     <t>qa.ram459@gmail.com</t>
   </si>
   <si>
@@ -36,13 +33,19 @@
     <t>cyclemg1@gmai</t>
   </si>
   <si>
-    <t>Buy</t>
-  </si>
-  <si>
     <t>search</t>
   </si>
   <si>
     <t>honda</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +440,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -456,17 +459,17 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
         <v>778</v>
@@ -479,36 +482,9 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -522,12 +498,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>